<commit_message>
Very small MLP for [2, 2, 2] starting point task
</commit_message>
<xml_diff>
--- a/experiments/pg/easy_simulation/traj_10_batch_100_max_rew_mlp_2x32_step_1e_1/log_best_traj.xlsx
+++ b/experiments/pg/easy_simulation/traj_10_batch_100_max_rew_mlp_2x32_step_1e_1/log_best_traj.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1241"/>
+  <dimension ref="A1:K1311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55278,6 +55278,3100 @@
         </is>
       </c>
     </row>
+    <row r="1242">
+      <c r="A1242" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1242" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>[2 2 2]</t>
+        </is>
+      </c>
+      <c r="D1242" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1242" t="n">
+        <v>15.91608409930835</v>
+      </c>
+      <c r="F1242" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1242" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1242" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1242" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1242" t="inlineStr">
+        <is>
+          <t>[0.9999991655349731, 6.687453435461066e-08, 6.651893613707216e-07]</t>
+        </is>
+      </c>
+      <c r="K1242" t="inlineStr">
+        <is>
+          <t>[1.0, 9.640592177703015e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1243" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>[1 2 2]</t>
+        </is>
+      </c>
+      <c r="D1243" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1243" t="n">
+        <v>23.26312162170652</v>
+      </c>
+      <c r="F1243" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1243" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1243" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1243" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1243" t="inlineStr">
+        <is>
+          <t>[3.4252884972829634e-08, 3.272637272289103e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1243" t="inlineStr">
+        <is>
+          <t>[1.0, 5.496145993571429e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1244" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>[1 2 1]</t>
+        </is>
+      </c>
+      <c r="D1244" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1244" t="n">
+        <v>19.01452196228093</v>
+      </c>
+      <c r="F1244" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1244" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1244" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1244" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1244" t="inlineStr">
+        <is>
+          <t>[3.9536356242466687e-19, 1.0, 1.4459463628605645e-13]</t>
+        </is>
+      </c>
+      <c r="K1244" t="inlineStr">
+        <is>
+          <t>[1.0, 4.281170205835986e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1245" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>[1 1 1]</t>
+        </is>
+      </c>
+      <c r="D1245" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1245" t="n">
+        <v>23.84833289025172</v>
+      </c>
+      <c r="F1245" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1245" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1245" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1245" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1245" t="inlineStr">
+        <is>
+          <t>[7.181615545304165e-12, 0.9999995231628418, 5.237781124378671e-07]</t>
+        </is>
+      </c>
+      <c r="K1245" t="inlineStr">
+        <is>
+          <t>[1.0, 2.0700967415831642e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1246" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>[1 0 1]</t>
+        </is>
+      </c>
+      <c r="D1246" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1246" t="n">
+        <v>23.35307809858611</v>
+      </c>
+      <c r="F1246" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1246" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1246" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1246" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1246" t="inlineStr">
+        <is>
+          <t>[3.527300951322587e-10, 1.070970670816445e-15, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1246" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0723389962944527e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1247" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>[1 0 0]</t>
+        </is>
+      </c>
+      <c r="D1247" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1247" t="n">
+        <v>24.25262015646103</v>
+      </c>
+      <c r="F1247" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1247" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1247" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1247" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1247" t="inlineStr">
+        <is>
+          <t>[5.454709600671848e-12, 1.0, 8.513431279388861e-12]</t>
+        </is>
+      </c>
+      <c r="K1247" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1721046709480446e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1248" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>[ 1 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1248" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1248" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="F1248" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1248" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1248" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1248" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1248" t="inlineStr">
+        <is>
+          <t>[0.9999990463256836, 8.173366268238169e-07, 1.1467574978496486e-07]</t>
+        </is>
+      </c>
+      <c r="K1248" t="inlineStr">
+        <is>
+          <t>[1.0, 7.56733113940459e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1249" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>[ 0 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1249" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1249" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1249" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1249" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1249" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1249" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1249" t="inlineStr">
+        <is>
+          <t>[3.1130173851028065e-13, 4.86989506498503e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1249" t="inlineStr">
+        <is>
+          <t>[1.0, 6.445454198739746e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1250" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>[ 0 -1 -1]</t>
+        </is>
+      </c>
+      <c r="D1250" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1250" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1250" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1250" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1250" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1250" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1250" t="inlineStr">
+        <is>
+          <t>[6.036733087830303e-15, 1.0, 1.667763908745623e-12]</t>
+        </is>
+      </c>
+      <c r="K1250" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1110056367463052e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1251" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>[ 0 -2 -1]</t>
+        </is>
+      </c>
+      <c r="D1251" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1251" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1251" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1251" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1251" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1251" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1251" t="inlineStr">
+        <is>
+          <t>[0.066717728972435, 0.9315569400787354, 0.0017253183759748936]</t>
+        </is>
+      </c>
+      <c r="K1251" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0811947919324454e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1252" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>[2 2 2]</t>
+        </is>
+      </c>
+      <c r="D1252" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1252" t="n">
+        <v>15.91608409930835</v>
+      </c>
+      <c r="F1252" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1252" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1252" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1252" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1252" t="inlineStr">
+        <is>
+          <t>[0.9999991655349731, 6.6147627819646e-08, 6.57748898902355e-07]</t>
+        </is>
+      </c>
+      <c r="K1252" t="inlineStr">
+        <is>
+          <t>[1.0, 9.640592177703015e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1253" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>[1 2 2]</t>
+        </is>
+      </c>
+      <c r="D1253" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1253" t="n">
+        <v>23.26312162170652</v>
+      </c>
+      <c r="F1253" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1253" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1253" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1253" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1253" t="inlineStr">
+        <is>
+          <t>[3.487540567448377e-08, 3.282984550878609e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1253" t="inlineStr">
+        <is>
+          <t>[1.0, 5.496145993571429e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1254" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>[1 2 1]</t>
+        </is>
+      </c>
+      <c r="D1254" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1254" t="n">
+        <v>19.01452196228093</v>
+      </c>
+      <c r="F1254" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1254" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1254" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1254" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1254" t="inlineStr">
+        <is>
+          <t>[3.993439813816662e-19, 1.0, 1.4466359154422653e-13]</t>
+        </is>
+      </c>
+      <c r="K1254" t="inlineStr">
+        <is>
+          <t>[1.0, 4.281170205835986e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1255" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>[1 1 1]</t>
+        </is>
+      </c>
+      <c r="D1255" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1255" t="n">
+        <v>23.84833289025172</v>
+      </c>
+      <c r="F1255" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1255" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1255" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1255" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1255" t="inlineStr">
+        <is>
+          <t>[7.284823785869143e-12, 0.9999995231628418, 5.226548864811775e-07]</t>
+        </is>
+      </c>
+      <c r="K1255" t="inlineStr">
+        <is>
+          <t>[1.0, 2.0700967415831642e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1256" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>[1 0 1]</t>
+        </is>
+      </c>
+      <c r="D1256" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1256" t="n">
+        <v>23.35307809858611</v>
+      </c>
+      <c r="F1256" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1256" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1256" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1256" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1256" t="inlineStr">
+        <is>
+          <t>[3.582417418268591e-10, 1.0711381715817645e-15, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1256" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0723389962944527e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1257" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>[1 0 0]</t>
+        </is>
+      </c>
+      <c r="D1257" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1257" t="n">
+        <v>24.25262015646103</v>
+      </c>
+      <c r="F1257" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1257" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1257" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1257" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1257" t="inlineStr">
+        <is>
+          <t>[5.521566710797732e-12, 1.0, 8.523049453701415e-12]</t>
+        </is>
+      </c>
+      <c r="K1257" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1721046709480446e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1258" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>[ 1 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1258" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1258" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="F1258" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1258" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1258" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1258" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1258" t="inlineStr">
+        <is>
+          <t>[0.9999990463256836, 8.028169418139441e-07, 1.127830415725839e-07]</t>
+        </is>
+      </c>
+      <c r="K1258" t="inlineStr">
+        <is>
+          <t>[1.0, 7.56733113940459e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1259" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>[ 0 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1259" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1259" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1259" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1259" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1259" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1259" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1259" t="inlineStr">
+        <is>
+          <t>[3.138492612499155e-13, 4.8538062458192144e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1259" t="inlineStr">
+        <is>
+          <t>[1.0, 6.445454198739746e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1260" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>[ 0 -1 -1]</t>
+        </is>
+      </c>
+      <c r="D1260" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1260" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1260" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1260" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1260" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1260" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1260" t="inlineStr">
+        <is>
+          <t>[6.085774601410432e-15, 1.0, 1.6646112656684697e-12]</t>
+        </is>
+      </c>
+      <c r="K1260" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1110056367463052e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="n">
+        <v>1250</v>
+      </c>
+      <c r="B1261" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>[ 0 -2 -1]</t>
+        </is>
+      </c>
+      <c r="D1261" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1261" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1261" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1261" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1261" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1261" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1261" t="inlineStr">
+        <is>
+          <t>[0.06762753427028656, 0.9306463599205017, 0.0017261207103729248]</t>
+        </is>
+      </c>
+      <c r="K1261" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0811947919324454e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1262" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>[2 2 2]</t>
+        </is>
+      </c>
+      <c r="D1262" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1262" t="n">
+        <v>15.91608409930835</v>
+      </c>
+      <c r="F1262" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1262" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1262" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1262" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1262" t="inlineStr">
+        <is>
+          <t>[0.9999992847442627, 6.542589403579768e-08, 6.503706231342221e-07]</t>
+        </is>
+      </c>
+      <c r="K1262" t="inlineStr">
+        <is>
+          <t>[1.0, 9.640592177703015e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1263" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>[1 2 2]</t>
+        </is>
+      </c>
+      <c r="D1263" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1263" t="n">
+        <v>23.26312162170652</v>
+      </c>
+      <c r="F1263" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1263" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1263" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1263" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1263" t="inlineStr">
+        <is>
+          <t>[3.5512016438588034e-08, 3.293514794222574e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1263" t="inlineStr">
+        <is>
+          <t>[1.0, 5.496145993571429e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1264" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>[1 2 1]</t>
+        </is>
+      </c>
+      <c r="D1264" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1264" t="n">
+        <v>19.01452196228093</v>
+      </c>
+      <c r="F1264" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1264" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1264" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1264" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1264" t="inlineStr">
+        <is>
+          <t>[4.033736692839007e-19, 1.0, 1.4473231640943496e-13]</t>
+        </is>
+      </c>
+      <c r="K1264" t="inlineStr">
+        <is>
+          <t>[1.0, 4.281170205835986e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1265" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>[1 1 1]</t>
+        </is>
+      </c>
+      <c r="D1265" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1265" t="n">
+        <v>23.84833289025172</v>
+      </c>
+      <c r="F1265" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1265" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1265" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1265" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1265" t="inlineStr">
+        <is>
+          <t>[7.389768484633574e-12, 0.9999995231628418, 5.215187002249877e-07]</t>
+        </is>
+      </c>
+      <c r="K1265" t="inlineStr">
+        <is>
+          <t>[1.0, 2.0700967415831642e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1266" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>[1 0 1]</t>
+        </is>
+      </c>
+      <c r="D1266" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1266" t="n">
+        <v>23.35307809858611</v>
+      </c>
+      <c r="F1266" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1266" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1266" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1266" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1266" t="inlineStr">
+        <is>
+          <t>[3.638707390951623e-10, 1.0713711056422595e-15, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1266" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0723389962944527e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1267" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>[1 0 0]</t>
+        </is>
+      </c>
+      <c r="D1267" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1267" t="n">
+        <v>24.25262015646103</v>
+      </c>
+      <c r="F1267" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1267" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1267" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1267" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1267" t="inlineStr">
+        <is>
+          <t>[5.589339321238063e-12, 1.0, 8.532580891840169e-12]</t>
+        </is>
+      </c>
+      <c r="K1267" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1721046709480446e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1268" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>[ 1 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1268" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1268" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="F1268" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1268" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1268" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1268" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1268" t="inlineStr">
+        <is>
+          <t>[0.9999990463256836, 7.88566524079215e-07, 1.1091596974210916e-07]</t>
+        </is>
+      </c>
+      <c r="K1268" t="inlineStr">
+        <is>
+          <t>[1.0, 7.56733113940459e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1269" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>[ 0 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1269" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1269" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1269" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1269" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1269" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1269" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1269" t="inlineStr">
+        <is>
+          <t>[3.1642906610923616e-13, 4.838065592593921e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1269" t="inlineStr">
+        <is>
+          <t>[1.0, 6.445454198739746e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1270" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>[ 0 -1 -1]</t>
+        </is>
+      </c>
+      <c r="D1270" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1270" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1270" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1270" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1270" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1270" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1270" t="inlineStr">
+        <is>
+          <t>[6.135167210147199e-15, 1.0, 1.6613949799237915e-12]</t>
+        </is>
+      </c>
+      <c r="K1270" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1110056367463052e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="n">
+        <v>1260</v>
+      </c>
+      <c r="B1271" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>[ 0 -2 -1]</t>
+        </is>
+      </c>
+      <c r="D1271" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1271" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1271" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1271" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1271" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1271" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1271" t="inlineStr">
+        <is>
+          <t>[0.06854809075593948, 0.929725170135498, 0.0017267819494009018]</t>
+        </is>
+      </c>
+      <c r="K1271" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0811947919324454e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1272" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>[2 2 2]</t>
+        </is>
+      </c>
+      <c r="D1272" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1272" t="n">
+        <v>15.91608409930835</v>
+      </c>
+      <c r="F1272" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1272" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1272" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1272" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1272" t="inlineStr">
+        <is>
+          <t>[0.9999992847442627, 6.470931168678362e-08, 6.430560119952133e-07]</t>
+        </is>
+      </c>
+      <c r="K1272" t="inlineStr">
+        <is>
+          <t>[1.0, 9.640592177703015e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1273" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>[1 2 2]</t>
+        </is>
+      </c>
+      <c r="D1273" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1273" t="n">
+        <v>23.26312162170652</v>
+      </c>
+      <c r="F1273" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1273" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1273" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1273" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1273" t="inlineStr">
+        <is>
+          <t>[3.616231936121039e-08, 3.3041228419961044e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1273" t="inlineStr">
+        <is>
+          <t>[1.0, 5.496145993571429e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1274" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>[1 2 1]</t>
+        </is>
+      </c>
+      <c r="D1274" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1274" t="n">
+        <v>19.01452196228093</v>
+      </c>
+      <c r="F1274" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1274" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1274" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1274" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1274" t="inlineStr">
+        <is>
+          <t>[4.074534274625888e-19, 1.0, 1.4479968602192778e-13]</t>
+        </is>
+      </c>
+      <c r="K1274" t="inlineStr">
+        <is>
+          <t>[1.0, 4.281170205835986e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1275" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>[1 1 1]</t>
+        </is>
+      </c>
+      <c r="D1275" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1275" t="n">
+        <v>23.84833289025172</v>
+      </c>
+      <c r="F1275" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1275" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1275" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1275" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1275" t="inlineStr">
+        <is>
+          <t>[7.496411477680986e-12, 0.9999995231628418, 5.203621071814268e-07]</t>
+        </is>
+      </c>
+      <c r="K1275" t="inlineStr">
+        <is>
+          <t>[1.0, 2.0700967415831642e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1276" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>[1 0 1]</t>
+        </is>
+      </c>
+      <c r="D1276" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1276" t="n">
+        <v>23.35307809858611</v>
+      </c>
+      <c r="F1276" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1276" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1276" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1276" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1276" t="inlineStr">
+        <is>
+          <t>[3.6961853022710045e-10, 1.0716776256900471e-15, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1276" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0723389962944527e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1277" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>[1 0 0]</t>
+        </is>
+      </c>
+      <c r="D1277" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1277" t="n">
+        <v>24.25262015646103</v>
+      </c>
+      <c r="F1277" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1277" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1277" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1277" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1277" t="inlineStr">
+        <is>
+          <t>[5.65791120551995e-12, 1.0, 8.541894622182689e-12]</t>
+        </is>
+      </c>
+      <c r="K1277" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1721046709480446e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1278" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>[ 1 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1278" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1278" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="F1278" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1278" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1278" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1278" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1278" t="inlineStr">
+        <is>
+          <t>[0.9999991655349731, 7.745735501885065e-07, 1.0907232450563242e-07]</t>
+        </is>
+      </c>
+      <c r="K1278" t="inlineStr">
+        <is>
+          <t>[1.0, 7.56733113940459e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1279" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>[ 0 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1279" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1279" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1279" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1279" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1279" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1279" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1279" t="inlineStr">
+        <is>
+          <t>[3.1905080248757767e-13, 4.8227899895891824e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1279" t="inlineStr">
+        <is>
+          <t>[1.0, 6.445454198739746e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1280" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>[ 0 -1 -1]</t>
+        </is>
+      </c>
+      <c r="D1280" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1280" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1280" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1280" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1280" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1280" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1280" t="inlineStr">
+        <is>
+          <t>[6.184842727888348e-15, 1.0, 1.6580931506277041e-12]</t>
+        </is>
+      </c>
+      <c r="K1280" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1110056367463052e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="n">
+        <v>1270</v>
+      </c>
+      <c r="B1281" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>[ 0 -2 -1]</t>
+        </is>
+      </c>
+      <c r="D1281" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1281" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1281" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1281" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1281" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1281" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1281" t="inlineStr">
+        <is>
+          <t>[0.0694783553481102, 0.9287943840026855, 0.0017272738041356206]</t>
+        </is>
+      </c>
+      <c r="K1281" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0811947919324454e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1282" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>[2 2 2]</t>
+        </is>
+      </c>
+      <c r="D1282" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1282" t="n">
+        <v>15.91608409930835</v>
+      </c>
+      <c r="F1282" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1282" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1282" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1282" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1282" t="inlineStr">
+        <is>
+          <t>[0.9999992847442627, 6.399862684247637e-08, 6.358078508128528e-07]</t>
+        </is>
+      </c>
+      <c r="K1282" t="inlineStr">
+        <is>
+          <t>[1.0, 9.640592177703015e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1283" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>[1 2 2]</t>
+        </is>
+      </c>
+      <c r="D1283" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1283" t="n">
+        <v>23.26312162170652</v>
+      </c>
+      <c r="F1283" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1283" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1283" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1283" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1283" t="inlineStr">
+        <is>
+          <t>[3.682572113916649e-08, 3.314816154897926e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1283" t="inlineStr">
+        <is>
+          <t>[1.0, 5.496145993571429e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1284" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>[1 2 1]</t>
+        </is>
+      </c>
+      <c r="D1284" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1284" t="n">
+        <v>19.01452196228093</v>
+      </c>
+      <c r="F1284" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1284" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1284" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1284" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1284" t="inlineStr">
+        <is>
+          <t>[4.115775173522309e-19, 1.0, 1.448640605259191e-13]</t>
+        </is>
+      </c>
+      <c r="K1284" t="inlineStr">
+        <is>
+          <t>[1.0, 4.281170205835986e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1285" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>[1 1 1]</t>
+        </is>
+      </c>
+      <c r="D1285" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1285" t="n">
+        <v>23.84833289025172</v>
+      </c>
+      <c r="F1285" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1285" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1285" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1285" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1285" t="inlineStr">
+        <is>
+          <t>[7.604622660750682e-12, 0.9999995231628418, 5.191872674004117e-07]</t>
+        </is>
+      </c>
+      <c r="K1285" t="inlineStr">
+        <is>
+          <t>[1.0, 2.0700967415831642e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1286" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>[1 0 1]</t>
+        </is>
+      </c>
+      <c r="D1286" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1286" t="n">
+        <v>23.35307809858611</v>
+      </c>
+      <c r="F1286" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1286" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1286" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1286" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1286" t="inlineStr">
+        <is>
+          <t>[3.7547995268560896e-10, 1.072029250242276e-15, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1286" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0723389962944527e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1287" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>[1 0 0]</t>
+        </is>
+      </c>
+      <c r="D1287" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1287" t="n">
+        <v>24.25262015646103</v>
+      </c>
+      <c r="F1287" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1287" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1287" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1287" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1287" t="inlineStr">
+        <is>
+          <t>[5.727335272709411e-12, 1.0, 8.551072176732344e-12]</t>
+        </is>
+      </c>
+      <c r="K1287" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1721046709480446e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1288" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>[ 1 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1288" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1288" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="F1288" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1288" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1288" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1288" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1288" t="inlineStr">
+        <is>
+          <t>[0.9999991655349731, 7.608272767356539e-07, 1.0725317167725734e-07]</t>
+        </is>
+      </c>
+      <c r="K1288" t="inlineStr">
+        <is>
+          <t>[1.0, 7.56733113940459e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1289" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>[ 0 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1289" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1289" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1289" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1289" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1289" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1289" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1289" t="inlineStr">
+        <is>
+          <t>[3.2170528177152824e-13, 4.8078558023689766e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1289" t="inlineStr">
+        <is>
+          <t>[1.0, 6.445454198739746e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1290" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>[ 0 -1 -1]</t>
+        </is>
+      </c>
+      <c r="D1290" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1290" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1290" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1290" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1290" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1290" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1290" t="inlineStr">
+        <is>
+          <t>[6.234801578150354e-15, 1.0, 1.6547221492330122e-12]</t>
+        </is>
+      </c>
+      <c r="K1290" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1110056367463052e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="n">
+        <v>1280</v>
+      </c>
+      <c r="B1291" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>[ 0 -2 -1]</t>
+        </is>
+      </c>
+      <c r="D1291" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1291" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1291" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1291" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1291" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1291" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1291" t="inlineStr">
+        <is>
+          <t>[0.07041938602924347, 0.9278530478477478, 0.0017276251455768943]</t>
+        </is>
+      </c>
+      <c r="K1291" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0811947919324454e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1292" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>[2 2 2]</t>
+        </is>
+      </c>
+      <c r="D1292" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1292" t="n">
+        <v>15.91608409930835</v>
+      </c>
+      <c r="F1292" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1292" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1292" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1292" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1292" t="inlineStr">
+        <is>
+          <t>[0.9999992847442627, 6.329309343300338e-08, 6.286150551204628e-07]</t>
+        </is>
+      </c>
+      <c r="K1292" t="inlineStr">
+        <is>
+          <t>[1.0, 9.640592177703015e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1293" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>[1 2 2]</t>
+        </is>
+      </c>
+      <c r="D1293" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1293" t="n">
+        <v>23.26312162170652</v>
+      </c>
+      <c r="F1293" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1293" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1293" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1293" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1293" t="inlineStr">
+        <is>
+          <t>[3.7504086947137694e-08, 3.325683195498641e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1293" t="inlineStr">
+        <is>
+          <t>[1.0, 5.496145993571429e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1294" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>[1 2 1]</t>
+        </is>
+      </c>
+      <c r="D1294" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1294" t="n">
+        <v>19.01452196228093</v>
+      </c>
+      <c r="F1294" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1294" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1294" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1294" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1294" t="inlineStr">
+        <is>
+          <t>[4.157512897774145e-19, 1.0, 1.4492789292882419e-13]</t>
+        </is>
+      </c>
+      <c r="K1294" t="inlineStr">
+        <is>
+          <t>[1.0, 4.281170205835986e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1295" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>[1 1 1]</t>
+        </is>
+      </c>
+      <c r="D1295" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1295" t="n">
+        <v>23.84833289025172</v>
+      </c>
+      <c r="F1295" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1295" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1295" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1295" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1295" t="inlineStr">
+        <is>
+          <t>[7.714542546444214e-12, 0.9999995231628418, 5.179899744689465e-07]</t>
+        </is>
+      </c>
+      <c r="K1295" t="inlineStr">
+        <is>
+          <t>[1.0, 2.0700967415831642e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1296" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>[1 0 1]</t>
+        </is>
+      </c>
+      <c r="D1296" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1296" t="n">
+        <v>23.35307809858611</v>
+      </c>
+      <c r="F1296" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1296" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1296" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1296" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1296" t="inlineStr">
+        <is>
+          <t>[3.814678573021979e-10, 1.0724628252321519e-15, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1296" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0723389962944527e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1297" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>[1 0 0]</t>
+        </is>
+      </c>
+      <c r="D1297" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1297" t="n">
+        <v>24.25262015646103</v>
+      </c>
+      <c r="F1297" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1297" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1297" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1297" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1297" t="inlineStr">
+        <is>
+          <t>[5.797666600276807e-12, 1.0, 8.560097075616113e-12]</t>
+        </is>
+      </c>
+      <c r="K1297" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1721046709480446e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1298" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>[ 1 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1298" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1298" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="F1298" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1298" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1298" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1298" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1298" t="inlineStr">
+        <is>
+          <t>[0.9999991655349731, 7.473263963220234e-07, 1.0545753781343592e-07]</t>
+        </is>
+      </c>
+      <c r="K1298" t="inlineStr">
+        <is>
+          <t>[1.0, 7.56733113940459e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1299" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>[ 0 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1299" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1299" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1299" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1299" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1299" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1299" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1299" t="inlineStr">
+        <is>
+          <t>[3.243954855170622e-13, 4.7932516622495314e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1299" t="inlineStr">
+        <is>
+          <t>[1.0, 6.445454198739746e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1300" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>[ 0 -1 -1]</t>
+        </is>
+      </c>
+      <c r="D1300" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1300" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1300" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1300" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1300" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1300" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1300" t="inlineStr">
+        <is>
+          <t>[6.28509204181121e-15, 1.0, 1.6512855536068849e-12]</t>
+        </is>
+      </c>
+      <c r="K1300" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1110056367463052e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="n">
+        <v>1290</v>
+      </c>
+      <c r="B1301" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>[ 0 -2 -1]</t>
+        </is>
+      </c>
+      <c r="D1301" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1301" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1301" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1301" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1301" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1301" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1301" t="inlineStr">
+        <is>
+          <t>[0.0713714212179184, 0.9269006848335266, 0.0017278454033657908]</t>
+        </is>
+      </c>
+      <c r="K1301" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0811947919324454e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1302" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>[2 2 2]</t>
+        </is>
+      </c>
+      <c r="D1302" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1302" t="n">
+        <v>15.91608409930835</v>
+      </c>
+      <c r="F1302" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1302" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1302" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1302" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1302" t="inlineStr">
+        <is>
+          <t>[0.9999992847442627, 6.259389806473337e-08, 6.21485867213778e-07]</t>
+        </is>
+      </c>
+      <c r="K1302" t="inlineStr">
+        <is>
+          <t>[1.0, 9.640592177703015e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1303" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>[1 2 2]</t>
+        </is>
+      </c>
+      <c r="D1303" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1303" t="n">
+        <v>23.26312162170652</v>
+      </c>
+      <c r="F1303" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1303" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1303" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1303" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1303" t="inlineStr">
+        <is>
+          <t>[3.819764415879945e-08, 3.336802478770551e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1303" t="inlineStr">
+        <is>
+          <t>[1.0, 5.496145993571429e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1304" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>[1 2 1]</t>
+        </is>
+      </c>
+      <c r="D1304" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1304" t="n">
+        <v>19.01452196228093</v>
+      </c>
+      <c r="F1304" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1304" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1304" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1304" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1304" t="inlineStr">
+        <is>
+          <t>[4.1997060883507676e-19, 1.0, 1.4498927232431402e-13]</t>
+        </is>
+      </c>
+      <c r="K1304" t="inlineStr">
+        <is>
+          <t>[1.0, 4.281170205835986e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1305" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>[1 1 1]</t>
+        </is>
+      </c>
+      <c r="D1305" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1305" t="n">
+        <v>23.84833289025172</v>
+      </c>
+      <c r="F1305" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1305" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1305" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1305" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1305" t="inlineStr">
+        <is>
+          <t>[7.826080929140833e-12, 0.9999995231628418, 5.167623839952284e-07]</t>
+        </is>
+      </c>
+      <c r="K1305" t="inlineStr">
+        <is>
+          <t>[1.0, 2.0700967415831642e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1306" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>[1 0 1]</t>
+        </is>
+      </c>
+      <c r="D1306" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1306" t="n">
+        <v>23.35307809858611</v>
+      </c>
+      <c r="F1306" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1306" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1306" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1306" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1306" t="inlineStr">
+        <is>
+          <t>[3.875837428779505e-10, 1.0729620452754399e-15, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1306" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0723389962944527e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1307" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>[1 0 0]</t>
+        </is>
+      </c>
+      <c r="D1307" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1307" t="n">
+        <v>24.25262015646103</v>
+      </c>
+      <c r="F1307" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1307" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1307" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1307" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1307" t="inlineStr">
+        <is>
+          <t>[5.8688613864543715e-12, 1.0, 8.568966716748783e-12]</t>
+        </is>
+      </c>
+      <c r="K1307" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1721046709480446e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1308" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>[ 1 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1308" t="inlineStr">
+        <is>
+          <t>[ 0 -1]</t>
+        </is>
+      </c>
+      <c r="E1308" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="F1308" t="n">
+        <v>2.574905395507812</v>
+      </c>
+      <c r="G1308" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1308" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1308" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1308" t="inlineStr">
+        <is>
+          <t>[0.9999991655349731, 7.340693741753057e-07, 1.0368484026912483e-07]</t>
+        </is>
+      </c>
+      <c r="K1308" t="inlineStr">
+        <is>
+          <t>[1.0, 7.56733113940459e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1309" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>[ 0 -1  0]</t>
+        </is>
+      </c>
+      <c r="D1309" t="inlineStr">
+        <is>
+          <t>[ 2 -1]</t>
+        </is>
+      </c>
+      <c r="E1309" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1309" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1309" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1309" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1309" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1309" t="inlineStr">
+        <is>
+          <t>[3.271181340126078e-13, 4.778965134732971e-08, 1.0]</t>
+        </is>
+      </c>
+      <c r="K1309" t="inlineStr">
+        <is>
+          <t>[1.0, 6.445454198739746e-18]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1310" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>[ 0 -1 -1]</t>
+        </is>
+      </c>
+      <c r="D1310" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1310" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1310" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1310" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1310" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1310" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1310" t="inlineStr">
+        <is>
+          <t>[6.335667532058817e-15, 1.0, 1.6477837974301912e-12]</t>
+        </is>
+      </c>
+      <c r="K1310" t="inlineStr">
+        <is>
+          <t>[1.0, 1.1110056367463052e-17]</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B1311" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>[ 0 -2 -1]</t>
+        </is>
+      </c>
+      <c r="D1311" t="inlineStr">
+        <is>
+          <t>[ 1 -1]</t>
+        </is>
+      </c>
+      <c r="E1311" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F1311" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G1311" t="n">
+        <v>25.74903836594053</v>
+      </c>
+      <c r="H1311" t="n">
+        <v>3.552713678800501e-15</v>
+      </c>
+      <c r="I1311" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="J1311" t="inlineStr">
+        <is>
+          <t>[0.07233335822820663, 0.9259386658668518, 0.0017279313178732991]</t>
+        </is>
+      </c>
+      <c r="K1311" t="inlineStr">
+        <is>
+          <t>[1.0, 1.0811947919324454e-17]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>